<commit_message>
Actualizando el módulo agregar productos
</commit_message>
<xml_diff>
--- a/productos_base.xlsx
+++ b/productos_base.xlsx
@@ -20,7 +20,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -54,6 +54,14 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -85,11 +93,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -105,12 +114,14 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Moneda [0]" xfId="1" builtinId="7"/>
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -268,8 +279,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TablaProductos" displayName="TablaProductos" ref="A1:AL10" headerRowCount="1" totalsRowShown="0">
-  <autoFilter ref="A1:AL8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TablaProductos" displayName="TablaProductos" ref="A1:AL23" headerRowCount="1" totalsRowShown="0">
+  <autoFilter ref="A1:AL23"/>
   <tableColumns count="38">
     <tableColumn id="1" name="ID" dataDxfId="8"/>
     <tableColumn id="2" name="Código de barra" dataDxfId="7"/>
@@ -636,10 +647,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL9"/>
+  <dimension ref="A1:AL22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="AD7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AI19" sqref="AI19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -652,22 +663,22 @@
     <col width="12.453125" customWidth="1" min="8" max="8"/>
     <col width="21.54296875" customWidth="1" min="10" max="10"/>
     <col width="44.26953125" customWidth="1" min="11" max="11"/>
-    <col width="14.7265625" customWidth="1" style="8" min="12" max="12"/>
-    <col width="10.90625" customWidth="1" style="8" min="13" max="13"/>
-    <col width="16.26953125" customWidth="1" style="8" min="14" max="14"/>
-    <col width="27.36328125" customWidth="1" style="8" min="15" max="15"/>
-    <col width="18.90625" customWidth="1" style="8" min="16" max="16"/>
-    <col width="20.36328125" customWidth="1" style="8" min="17" max="17"/>
-    <col width="25.54296875" customWidth="1" style="8" min="18" max="18"/>
-    <col width="19.81640625" customWidth="1" style="8" min="19" max="19"/>
-    <col width="23" customWidth="1" style="8" min="20" max="20"/>
-    <col width="42.1796875" customWidth="1" style="8" min="21" max="21"/>
-    <col width="32.453125" customWidth="1" style="8" min="22" max="22"/>
-    <col width="37.26953125" customWidth="1" style="8" min="23" max="23"/>
-    <col width="33.81640625" customWidth="1" style="8" min="24" max="24"/>
-    <col width="37" customWidth="1" style="8" min="25" max="25"/>
-    <col width="46.7265625" customWidth="1" style="8" min="26" max="26"/>
-    <col width="23.453125" customWidth="1" style="8" min="27" max="27"/>
+    <col width="14.7265625" customWidth="1" style="9" min="12" max="12"/>
+    <col width="10.90625" customWidth="1" style="9" min="13" max="13"/>
+    <col width="16.26953125" customWidth="1" style="9" min="14" max="14"/>
+    <col width="27.36328125" customWidth="1" style="9" min="15" max="15"/>
+    <col width="18.90625" customWidth="1" style="9" min="16" max="16"/>
+    <col width="20.36328125" customWidth="1" style="9" min="17" max="17"/>
+    <col width="25.54296875" customWidth="1" style="9" min="18" max="18"/>
+    <col width="19.81640625" customWidth="1" style="9" min="19" max="19"/>
+    <col width="23" customWidth="1" style="9" min="20" max="20"/>
+    <col width="42.1796875" customWidth="1" style="9" min="21" max="21"/>
+    <col width="32.453125" customWidth="1" style="9" min="22" max="22"/>
+    <col width="37.26953125" customWidth="1" style="9" min="23" max="23"/>
+    <col width="33.81640625" customWidth="1" style="9" min="24" max="24"/>
+    <col width="37" customWidth="1" style="9" min="25" max="25"/>
+    <col width="46.7265625" customWidth="1" style="9" min="26" max="26"/>
+    <col width="23.453125" customWidth="1" style="9" min="27" max="27"/>
     <col width="19.54296875" customWidth="1" min="28" max="28"/>
     <col width="26.90625" customWidth="1" min="29" max="29"/>
     <col width="17.453125" customWidth="1" min="30" max="33"/>
@@ -733,82 +744,82 @@
           <t>Imágenes secundarias (URLs separadas por coma)</t>
         </is>
       </c>
-      <c r="L1" s="8" t="inlineStr">
+      <c r="L1" s="9" t="inlineStr">
         <is>
           <t>Precio compra</t>
         </is>
       </c>
-      <c r="M1" s="8" t="inlineStr">
+      <c r="M1" s="9" t="inlineStr">
         <is>
           <t>Stock</t>
         </is>
       </c>
-      <c r="N1" s="8" t="inlineStr">
+      <c r="N1" s="9" t="inlineStr">
         <is>
           <t>Precio Facebook</t>
         </is>
       </c>
-      <c r="O1" s="8" t="inlineStr">
+      <c r="O1" s="9" t="inlineStr">
         <is>
           <t>Comisión vendedor Facebook</t>
         </is>
       </c>
-      <c r="P1" s="8" t="inlineStr">
+      <c r="P1" s="9" t="inlineStr">
         <is>
           <t>Ganancia Facebook</t>
         </is>
       </c>
-      <c r="Q1" s="8" t="inlineStr">
+      <c r="Q1" s="9" t="inlineStr">
         <is>
           <t>Precio Mercado Libre</t>
         </is>
       </c>
-      <c r="R1" s="8" t="inlineStr">
+      <c r="R1" s="9" t="inlineStr">
         <is>
           <t>Comisión de Mercado Libre</t>
         </is>
       </c>
-      <c r="S1" s="8" t="inlineStr">
+      <c r="S1" s="9" t="inlineStr">
         <is>
           <t>Envio Mercado Libre</t>
         </is>
       </c>
-      <c r="T1" s="8" t="inlineStr">
+      <c r="T1" s="9" t="inlineStr">
         <is>
           <t>Ganancia Mercado Libre</t>
         </is>
       </c>
-      <c r="U1" s="8" t="inlineStr">
+      <c r="U1" s="9" t="inlineStr">
         <is>
           <t>Ganancia de Mercado Libre despues de iva 19%</t>
         </is>
       </c>
-      <c r="V1" s="8" t="inlineStr">
+      <c r="V1" s="9" t="inlineStr">
         <is>
           <t>Precio Mercado Libre con 30% desc.</t>
         </is>
       </c>
-      <c r="W1" s="8" t="inlineStr">
+      <c r="W1" s="9" t="inlineStr">
         <is>
           <t>Comisión de Mercado libre con 30% desc.</t>
         </is>
       </c>
-      <c r="X1" s="8" t="inlineStr">
+      <c r="X1" s="9" t="inlineStr">
         <is>
           <t>Envio Mercado Libre con el 30% desc.</t>
         </is>
       </c>
-      <c r="Y1" s="8" t="inlineStr">
+      <c r="Y1" s="9" t="inlineStr">
         <is>
           <t>Ganancia Mercado Libre con el 30% desc.</t>
         </is>
       </c>
-      <c r="Z1" s="8" t="inlineStr">
+      <c r="Z1" s="9" t="inlineStr">
         <is>
           <t>Ganancia de Mercado Libre despues de iva 19% con el 30% desc.</t>
         </is>
       </c>
-      <c r="AA1" s="8" t="inlineStr">
+      <c r="AA1" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Precio al por mayor de 3 </t>
         </is>
@@ -875,8 +886,10 @@
           <t>P003</t>
         </is>
       </c>
-      <c r="B2" s="5" t="n">
-        <v>6900822110052</v>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>6900822110052</t>
+        </is>
       </c>
       <c r="C2" s="6" t="inlineStr">
         <is>
@@ -942,53 +955,85 @@
           <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1743601960/11_on8xob.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1743601960/10_v630x9.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1743601960/4_p5fbwz.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1743601960/3_fjc1gt.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1743601960/5_b58to6.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1743601961/9_v5lnv4.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1743601961/2_cgojj6.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1743601961/8_frlrfn.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1743601961/7_s6qyap.jpg,</t>
         </is>
       </c>
-      <c r="L2" s="8" t="n">
-        <v>4900</v>
-      </c>
-      <c r="M2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" s="8" t="n">
-        <v>7990</v>
-      </c>
-      <c r="O2" s="8" t="n">
-        <v>1500</v>
-      </c>
-      <c r="P2" s="8" t="n">
-        <v>1590</v>
-      </c>
-      <c r="Q2" s="8" t="n">
-        <v>15700</v>
-      </c>
-      <c r="R2" s="8" t="n">
-        <v>3355</v>
-      </c>
-      <c r="S2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" s="8" t="n">
-        <v>7445</v>
-      </c>
-      <c r="U2" s="8" t="n">
-        <v>5099</v>
-      </c>
-      <c r="V2" s="8" t="n">
-        <v>10990</v>
-      </c>
-      <c r="W2" s="8" t="n">
-        <v>2648</v>
-      </c>
-      <c r="X2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="8" t="n">
-        <v>3442</v>
-      </c>
-      <c r="Z2" s="8" t="n">
-        <v>1875</v>
-      </c>
-      <c r="AA2" s="8" t="n">
-        <v>6500</v>
+      <c r="L2" s="9" t="inlineStr">
+        <is>
+          <t>4900</t>
+        </is>
+      </c>
+      <c r="M2" s="9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N2" s="9" t="inlineStr">
+        <is>
+          <t>7990</t>
+        </is>
+      </c>
+      <c r="O2" s="9" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="P2" s="9" t="inlineStr">
+        <is>
+          <t>1590</t>
+        </is>
+      </c>
+      <c r="Q2" s="9" t="inlineStr">
+        <is>
+          <t>15700.0</t>
+        </is>
+      </c>
+      <c r="R2" s="9" t="inlineStr">
+        <is>
+          <t>3355.0</t>
+        </is>
+      </c>
+      <c r="S2" s="9" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="T2" s="9" t="inlineStr">
+        <is>
+          <t>7445.0</t>
+        </is>
+      </c>
+      <c r="U2" s="9" t="inlineStr">
+        <is>
+          <t>5099.0</t>
+        </is>
+      </c>
+      <c r="V2" s="9" t="inlineStr">
+        <is>
+          <t>10990.0</t>
+        </is>
+      </c>
+      <c r="W2" s="9" t="inlineStr">
+        <is>
+          <t>2648.0</t>
+        </is>
+      </c>
+      <c r="X2" s="9" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="Y2" s="9" t="inlineStr">
+        <is>
+          <t>3442.0</t>
+        </is>
+      </c>
+      <c r="Z2" s="9" t="inlineStr">
+        <is>
+          <t>1875.0</t>
+        </is>
+      </c>
+      <c r="AA2" s="9" t="inlineStr">
+        <is>
+          <t>6500</t>
+        </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
@@ -1005,6 +1050,12 @@
           <t>https://www.mercadolibre.cl/lampara-luz-nocturna-fantasma-silicona-luz-nocturna-infantil/up/MLCU3103906632</t>
         </is>
       </c>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="inlineStr">
         <is>
           <t>lámpara fantasma, luz nocturna niños, lámpara silicona, lámpara recargable, lámpara infantil, luz de noche, regalo niños, luz escritorio, decoración infantil, luz fantasma, lámpara LED, luz LED portátil, regalo para dormir, juguete antiestrés, lámpara con temporizador, luz regulable, lámpara kawaii, luz para bebés, lámpara para regalo</t>
@@ -2272,12 +2323,6 @@
           <t>http://mercadolibre.cl/peluche-elefante-suave-de-25cm-para-ninos-y-bebes-gris/up/MLCU3106924924</t>
         </is>
       </c>
-      <c r="AE9" t="inlineStr"/>
-      <c r="AF9" t="inlineStr"/>
-      <c r="AG9" t="inlineStr"/>
-      <c r="AH9" t="inlineStr"/>
-      <c r="AI9" t="inlineStr"/>
-      <c r="AJ9" t="inlineStr"/>
       <c r="AK9" t="inlineStr">
         <is>
           <t>peluche elefante, elefante de peluche, peluche infantil, peluche suave, juguete para bebé, regalo baby shower, peluche gris, muñeco de peluche, peluche 25 cm, juguete niño 3 años, animal de peluche, peluche algodón, peluche orejas grandes, elefante tierno, peluche decorativo, peluche sin batería, muñeco seguro, juguete suave, peluche compacto, peluche pequeño</t>
@@ -2286,14 +2331,2013 @@
       <c r="AL9" t="inlineStr">
         <is>
           <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1743702273/Milestar_qtk5mw.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>P011</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>6923292231850</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>6923292231850</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Milestar</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Peluche Elefante Rosado Suave con Moño 25cm para Niñas</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Juguetes</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Montelameda</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🐘 **Peluche Elefante Rosado Suave con Moño 25cm para Niñas**
+Este adorable **elefante rosado de peluche** es el compañero perfecto para niñas. Con un diseño tierno y detalles encantadores como su moño en la oreja, se convierte en un regalo ideal para cumpleaños, baby showers o simplemente para decorar una habitación infantil.
+ ✨ **Descripción:**
+¡Dale color y ternura al espacio de tu pequeña! Este peluche elefante tiene un diseño femenino, suave y cómodo al tacto. Sus colores pastel, orejitas grandes y moñito decorativo lo hacen irresistible. Además, su tamaño de **25x21.5 cm** es perfecto para abrazar, jugar o llevar de paseo.
+🎁 Ideal para:
+- Regalo de cumpleaños o Día del Niño
+- Decoración de dormitorio infantil
+- Muñeco de apego para bebés
+- Detalle especial para recién nacidas
+ 📋 **Ficha Técnica**
+- **Producto:** Peluche Elefante Rosado con Moño
+- **Color:** Rosado con detalles grises
+- **Dimensiones:** 25 cm (largo) x 21.5 cm (alto)
+- **Material:** Felpa ultra suave con relleno de algodón PP
+- **Peso estimado:** 200 g
+- **Edad recomendada:** Desde los 3 años
+- **Baterías requeridas:** No
+- **Incluye baterías:** No
+- **Montaje necesario:** No
+- **Uso:** Decoración, juego, regalo
+</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Nuevo</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1743702019/1_lsfqgw.jpg</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1743702020/2_zg79ev.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1743702020/3_tmtrpe.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1743702021/4_rhsaix.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1743702022/5_ezybb0.jpg</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>6990</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>2768</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>11414</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>2826</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>5366</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>3734</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>7990</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>1978</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>2790</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>1648</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>5500</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>#159440874</t>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>https://www.mercadolibre.cl/peluche-elefante-rosado-suave-con-mono-25cm-para-ninas/up/MLCU3108532236</t>
+        </is>
+      </c>
+      <c r="AK10" t="inlineStr">
+        <is>
+          <t>peluche elefante rosado, peluche con moño, elefante de peluche, muñeco rosado, regalo para niña, peluche decorativo, peluche infantil, peluche bebé, juguete niña, peluche 25 cm, peluche suave, muñeco tierno, felpa rosada, peluche orejas grandes, muñeco para abrazar, peluche algodón, peluche regalo niña, peluche cumpleaños, peluche tierno rosa, peluche moño</t>
+        </is>
+      </c>
+      <c r="AL10" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1743702023/Milestar_opjvxm.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>P012</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>8445904021065</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>8445904021065</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Milestar</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Peluche Dinosaurio 26cm Suave Decoración Juguete Niños</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Juguetes</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Montelameda</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🦖 ¡Llega el compañero más adorable para grandes y chicos!
+Este **peluche de dinosaurio de 26 cm** es perfecto para abrazar, jugar o decorar. Su diseño tierno y su textura extra suave lo hacen irresistible para cualquier edad. Ideal para regalar, coleccionar o usar como decoración en habitaciones infantiles.
+💡 *El modelo se envía según disponibilidad* — ¡todos son igual de adorables, no hay pierde! 😍
+### ✅ **¿Por qué te encantará?**
+- Hecho con materiales suaves y de calidad
+- Ligero, esponjoso y muy agradable al tacto
+- Diseño kawaii con detalles bordados
+- Excelente opción para cumpleaños, baby showers o sorpresas espontáneas
+### 📋 **Ficha Técnica:**
+- **Producto:** Peluche Dinosaurio  
+- **Altura:** 26 cm  
+- **Material:** Felpa suave + relleno de algodón PP  
+- **Peso:** Aprox. 200 g  
+- **Colores:** Varían según disponibilidad  
+- **Edad recomendada:** 3 años en adelante  
+- **Usos:** Juguete, decoración, regalo  
+</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Nuevo</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1743702014/1_rm6wov.jpg</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1743702015/3_mxebpf.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1743702015/2_gfb75m.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1743702017/5_odi9ru.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1743702016/4_tjdyhl.jpg</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>4222</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>7990</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>2768</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>12843</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>3055</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>5566</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>3706</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>8990</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>2138</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>2630</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>1328</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>5990</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>#1594292529</t>
+        </is>
+      </c>
+      <c r="AD11" s="7" t="inlineStr">
+        <is>
+          <t>https://www.mercadolibre.cl/peluche-dinosaurio-26cm-suave-decoracion-juguete-ninos/up/MLCU3103200281?pdp_filters=item_id:MLC1594292529</t>
+        </is>
+      </c>
+      <c r="AK11" t="inlineStr">
+        <is>
+          <t>peluche dinosaurio, peluche suave, juguete dinosaurio, muñeco tierno, regalo infantil, peluche 26 cm, peluche bebé, dinosaurio para niños, decoración infantil, peluche kawaii, muñeco abrazable, juguete tierno, dinosaurio de felpa, muñeco suave, peluche niño, peluche regalo, peluche coleccionable, peluche verde, peluche felpa, peluche de animal</t>
+        </is>
+      </c>
+      <c r="AL11" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1743702018/Milestar_nig4e6.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>P013</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>7858816135507</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>13550</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>IRM</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Lámpara de Noche Capibara Recargable Cambia de Colores</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Hogar</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Montelameda</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">✨ ¡Dale un toque adorable y relajante a tu espacio con esta lámpara de noche con forma de capibara! 🦫 Perfecta para niños y adultos, cambia de colores con el movimiento y ofrece una luz suave y acogedora ideal para dormir. 🌈  
+🛠️ **Características destacadas:**  
+- **Función de apagado automático:** Se apaga en 30 minutos o funciona hasta agotar la batería.  
+- **Cambia de colores:** Responde al movimiento para crear un ambiente único.  
+- **Recargable por USB:** Incluye cable USB para mayor comodidad.  
+- **Material suave y seguro:** Hecho de goma flexible y agradable al tacto.  
+- **Tamaño compacto:** 13 cm de alto x 8.5 cm de ancho.  
+🎁 **Beneficios:**  
+- Perfecta para acompañar las noches de los niños.  
+- Proporciona un ambiente relajante para dormir.  
+- Fácil de usar y transportar.  
+- Ideal como regalo decorativo y funcional.  
+### **Ficha técnica:**  
+- **Material:** Goma suave y segura.  
+- **Dimensiones:** 13 cm de alto x 8.5 cm de ancho.  
+- **Tipo de luz:** LED multicolor con cambio por movimiento.  
+- **Alimentación:** Recargable vía USB (cable incluido).  
+- **Modos de funcionamiento:**  
+  - Apagado automático a los 30 minutos.  
+  - Modo continuo hasta agotar la batería.  
+- **Uso recomendado:** Habitación, noche, regalo infantil.  
+</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Nuevo</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744044461/1_oonsgy.png</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744044486/Photoroom-20241215_163954_ofwcuz.png,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744044463/6_c67png.png,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744044463/9_upfrlp.png,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744044462/7_tfxftu.png,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744044461/3_k4tfxe.png,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744044461/10_dgvkeq.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744044460/12_scryvc.webp,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744044460/11_bnoxas.webp</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>3900</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>7990</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>3090</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>12843</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>2926</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>6017</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>4133</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>8990</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>2049</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>3041</t>
+        </is>
+      </c>
+      <c r="Z12" t="inlineStr">
+        <is>
+          <t>1722</t>
+        </is>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>5990</t>
+        </is>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>#1573152315</t>
+        </is>
+      </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>https://articulo.mercadolibre.cl/MLC-1573152315-lampara-luz-nocturna-de-capibara-lampara-de-noche-colores-_JM</t>
+        </is>
+      </c>
+      <c r="AK12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">lámpara de noche, capibara luz nocturna, lámpara infantil, luz LED recargable, luz decorativa, lámpara cambia colores, regalo para niños, luz con apagado automático, luz nocturna USB, lámpara de goma, ambiente relajante, lámpara capibara, iluminación suave, juguete de luz, luz para dormir, lámpara recargable, luz LED para habitación, luz compacta, decoración infantil, accesorio de noche.  </t>
+        </is>
+      </c>
+      <c r="AL12" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744044850/IRM_j3ujao.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>P014</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>78027</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>78027</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Doremi</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Juguete Diábolo Mediano 2 Varilla Y 1 Cuerda Malabares Yoyo</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Juguetes</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Montelameda</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+🎯 **Diábolo de Madera - Yoyo Chino Clásico para Todas las Edades** 🎯
+🪀 **Diversión sin límites**: El diábolo de madera es un juguete tradicional que desafía la destreza y la coordinación de niños, jóvenes y adultos. ¡Perfecto para practicar trucos y mejorar la motricidad fina!
+🌳 **Materiales respetuosos con el medio ambiente**: Fabricado con una combinación de madera y plástico de alta calidad, este diábolo es ligero, resistente y seguro para jugar tanto en interiores como exteriores.
+⚖️ **Equilibrio perfecto**: Su diseño clásico asegura un excelente equilibrio, facilitando el aprendizaje de movimientos y acrobacias. Ideal para principiantes y jugadores intermedios.
+🎉 **Horas de entretenimiento aseguradas**: Adecuado para todas las edades, este juguete puede ayudar a mejorar la coordinación de manos y brazos, mientras ofrece una experiencia divertida.
+✨ **Duradero y resistente**: El diábolo está diseñado para soportar caídas sin romperse, ¡perfecto para quienes recién están aprendiendo!
+📦 **Contenido del paquete**:
+- 1 Diábolo de madera
+- 2 Palos de control
+🔒 **Seguro y ecológico**: Materiales aptos para el uso continuo y respetuosos con el medio ambiente, para que disfrutes sin preocupaciones.
+### 3. **Ficha técnica:**
+- **Tipo**: Diábolo de madera (Yoyo chino)
+- **Materiales**: Madera y plástico
+- **Adecuado para**: Todas las edades, principiantes e intermedios
+- **Uso**: Interior y exterior
+- **Características**: Ligero, duradero, respetuoso con el medio ambiente
+</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Nuevo</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744045187/1_fqwrp9.jpg</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744045187/3_jxas5z.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744045187/10_s90pcn.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744045187/2_lhmtku.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744045188/4_gwzyxe.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744045188/5_jkcbib.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744045189/6_iebuui.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744045190/8_zd0geu.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744045190/7_sejpwr.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744045191/9_eofjad.jpg</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>2600</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>4990</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>1390</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>8557</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>1659</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>4298</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>2987</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>5990</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>1659</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>1731</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>908</t>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>3990</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>#2851993410</t>
+        </is>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>https://www.mercadolibre.cl/juguete-diabolo-mediano-2-varilla-y-1-cuerda-malabares-yoyo/up/MLCU3049219268?pdp_filters=item_id:MLC2851993410</t>
+        </is>
+      </c>
+      <c r="AK13" t="inlineStr">
+        <is>
+          <t>diábolo de madera, yoyo chino, juego de habilidad, diábolo para principiantes, juguete clásico, diábolo para niños, juguete ecológico, diábolo resistente, juguete tradicional, diábolo para adultos, diábolo de colores, juguete de coordinación, juego de trucos, juguete de equilibrio, yoyo de madera, diábolo exterior, diábolo interior, juguete de destreza, diábolo con palos, yoyo chino de madera</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>P015</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2824</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2824</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>El Salto</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Caballito de palo con Sonido y rueda de 100 cm para Niño</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Juguetes</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Montelameda</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">*🏇 **Caballo Bastón con Sonido** - ¡La diversión está asegurada con este encantador caballito con bastón y sonido! Ideal para pequeños jinetes llenos de energía, este juguete es perfecto para estimular la imaginación y promover el juego activo.
+🔊 **Función de Sonido**: La oreja de la cabeza de caballo de felpa activa un sonido de galope y aullido, proporcionando una experiencia de juego más realista y divertida. ¡Fácil de encender y apagar!
+📏 **Dimensiones y Peso**:
+- **Tamaño del Caballo**: Aproximadamente 100 x 22 x 27 cm
+- **Peso del Caballo**: Aproximadamente 380 g
+- **Longitud de las Asas**: 6 cm
+🎨 **Colores Disponibles**: Negro, Marrón, Crema
+🚸 **Seguridad y Normativa**:
+- Juguete no tóxico que cumple con la normativa Chilena.
+- Recomendado para niños mayores de 3 años.
+Este caballito con bastón es una excelente opción para regalar en cumpleaños, navidades, o simplemente para alegrar el día a día de los más pequeños. ¡Haz que la diversión y la aventura lleguen a tu hogar!
+---
+### Ficha Técnica:
+- **Nombre del Producto**: Caballo Bastón con Sonido
+- **Material**: Felpa y madera
+- **Dimensiones del Producto**: 100 x 22 x 27 cm
+- **Peso del Producto**: 380 g
+- **Longitud de las Asas**: 6 cm
+- **Colores Disponibles**: Negro, Marrón, Crema
+- **Edad Recomendada**: 3 años en adelante
+- **Normativa**: Juguete no tóxico que cumple con la normativa Chilena
+</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Nuevo</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744046209/1_ezv8pw.jpg</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744046208/3_euwbj8.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744046208/2_yxeixc.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744046273/4_fppagc.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744046273/10_jt94xh.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744046273/10_jt94xh.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744046274/9_vvwsfp.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744046275/5_zwwe28.jpg</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>7500</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>14990</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>5990</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>22843</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>3654</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>3100</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>8589</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>5532</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>15990</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>3559</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>4931</t>
+        </is>
+      </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t>2569</t>
+        </is>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>11990</t>
+        </is>
+      </c>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>#1578814137</t>
+        </is>
+      </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>https://articulo.mercadolibre.cl/MLC-1578814137-caballito-de-palo-con-sonido-y-rueda-de-100-cm-para-ninos-_JM</t>
+        </is>
+      </c>
+      <c r="AK14" t="inlineStr">
+        <is>
+          <t>caballo bastón, juguete con sonido, caballo de felpa, juguete para niños, caballito con sonido, juguete activo, regalo para niños, juego imaginativo, caballo de palo, juguete no tóxico, caballito de juguete, juguete de aventura, juego al aire libre, regalo infantil, juguete seguro, caballito para montar, juguetes educativos, caballo de juguete, caballito con bastón, diversión para niños</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>P016</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>51161</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>51161</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>IRM</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Cable de Carga Rápida 3 en 1 Lightning Tipo C y Micro USB</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Tecnología</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Montelameda</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+📝 Descripción: "🌟 Mejora tu experiencia de carga con el Cable 3 en 1 VIDVIE. Diseñado con un recubrimiento trenzado duradero y conexiones para iPhone, Android y dispositivos USB-C, es perfecto para cualquier dispositivo. 🚀 Disfruta de carga rápida de 3A y una longitud de 120 cm que te da flexibilidad. Compatible con los principales modelos de smartphones y tablets.
+Ideal para el hogar, oficina o llevar de viaje. ¡No te quedes sin batería! 🔌🔋
+📏 Longitud: 120 cm ⚡ Carga rápida: 3A 🔗 Conectores: USB-C, micro USB, lightning 💪 Material: Nylon trenzado de alta resistencia"
+📋 Ficha técnica:
+Material: Nylon trenzado
+Longitud: 120 cm
+Corriente máxima: 3A
+Conectores: USB-C, micro USB, lightning
+Compatibilidad: iOS, Android
+Color: Negro
+</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Nuevo</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744057581/3_tzeluj.jpg</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744057581/5_yrgh28.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744057581/4_psksce.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744057581/1_f6x8x2.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744057581/2_pg8k5t.jpg</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>1900</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>4990</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>2090</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>7129</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>1627</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>3602</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>2557</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>4990</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>1349</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>1741</t>
+        </is>
+      </c>
+      <c r="Z15" t="inlineStr">
+        <is>
+          <t>1049</t>
+        </is>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>3990</t>
+        </is>
+      </c>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>#1595390341</t>
+        </is>
+      </c>
+      <c r="AD15" s="7" t="inlineStr">
+        <is>
+          <t>https://www.mercadolibre.cl/cable-de-carga-rapida-3-en-1-lightning-tipo-c-y-micro-usb/up/MLCU3107934351</t>
+        </is>
+      </c>
+      <c r="AK15" t="inlineStr">
+        <is>
+          <t>cable 3 en 1, carga rápida, cable VIDVIE, USB-C, micro USB, lightning, cable trenzado, 120 cm, alta resistencia, carga múltiple, cable universal, tecnología, accesible y práctico, cargador multifuncional, accesorios móviles, gadgets, compatibilidad Android y iOS, cable duradero, tecnología de carga rápida</t>
+        </is>
+      </c>
+      <c r="AL15" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744057628/IRM_youd3d.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>P017</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>7858816011016</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1101</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>IRM</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Cargador universal para notebook 120W con 9 conectores</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Tecnología</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Montelameda</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+📝 Descripción: ** Descubre el potente cargador universal de 120W para notebooks, ideal para cualquier laptop gracias a sus 9 conectores adaptables. 🌟 Compatible con voltajes de 12-24V, es perfecto para mantener tus dispositivos siempre cargados. Con un diseño compacto y ligero, llévalo a donde quieras. 💼
+📋 Ficha técnica:
+**
+Potencia: 120W
+Voltaje de entrada: 12-24V
+Incluye 9 conectores intercambiables
+Compatible con la mayoría de los notebooks
+Diseño compacto y portátil
+</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Nuevo</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744057741/3_d5yrqn.jpg</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744057741/4_ye1zfm.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744057780/5_zzwqn2.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744057740/1_fjhibq.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744057741/2_owcada.jpg</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>4900</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>7990</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>2090</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>15700</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>3041</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>7759</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>5354</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>10990</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>2429</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>3661</t>
+        </is>
+      </c>
+      <c r="Z16" t="inlineStr">
+        <is>
+          <t>2034</t>
+        </is>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>6990</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>#2868263222</t>
+        </is>
+      </c>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>https://www.mercadolibre.cl/cargador-universal-para-notebook-120w-con-9-conectores/up/MLCU3107967751</t>
+        </is>
+      </c>
+      <c r="AK16" t="inlineStr">
+        <is>
+          <t>cargador universal, notebook, adaptador múltiple, 120W, portátil, laptop, conectores múltiples, MeidiMake, IRM, adaptador notebook, accesorio laptop, cargador compacto, cargador portátil, potencia 120W, cargador conector, adaptador universal, multi-conexión, cargador seguro, cargador versátil, tecnología adaptador, accesorio computadora</t>
+        </is>
+      </c>
+      <c r="AL16" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744057924/IRM_hyvmd6.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>P018</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>7858816136047</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>13604</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>IRM</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Control Remoto Universal RM 1869 para TV</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Tecnología</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Montelameda</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Descripción: " Control Remoto Universal RM-1869  Compatible con 94 marcas de televisores . Simplemente inserta las baterías y ¡listo! Controla funciones esenciales y accede a tus plataformas favoritas como NET TV y PRIME V. Ideal para reemplazo o como control adicional.
+Tamaño compacto: 19.5 cm x 4.3 cm
+Funcionalidad completa con acceso rápido 
+Diseño ergonómico y duradero  No te quedes sin control y mejora tu experiencia de visualización."
+ Ficha técnica:
+Modelo: RM-1869
+Compatibilidad: 94 marcas de TV
+Dimensiones: 19.5 cm x 4.3 cm
+Material: Plástico resistente
+Alimentación: Pilas (no incluidas)
+</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Nuevo</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058196/6_vfjti3.jpg</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744057972/1_p4flwo.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058195/3_cswzm7.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058196/2_wl6hzg.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058196/5_i43ri4.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058196/4_kl94xa.jpg,</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>2700</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>5990</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>2290</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>9986</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>2298</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>4988</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>3527</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>6990</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>1818</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>2472</t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>1489</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>4990</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>#1595454983</t>
+        </is>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>https://www.mercadolibre.cl/control-remoto-universal--para-tv/up/MLCU3113403104</t>
+        </is>
+      </c>
+      <c r="AK17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> control remoto, universal, TV, MeidiMake, RM-1869, mando a distancia, televisor, reemplazo, fácil uso, multicompatible, botones, ergonomía, diseño compacto, funcional, acceso rápido, NET TV, PRIME V, accesorio TV, comodidad.</t>
+        </is>
+      </c>
+      <c r="AL17" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058195/2_vuei1g.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>P019</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>785881613644</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>13644</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Kit Cortadora de Cabello Eléctrica Modelo 717</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Salud e Higiene</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Montelameda</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+📝 Descripción: ** ¡Transforma tu look desde casa! 🌟 Con el Kit Cortadora de Cabello IRM Modelo 717, tienes todo lo que necesitas para un corte preciso y profesional. Incluye una potente cortadora eléctrica, peines guía para distintas longitudes, tijeras, peine y aceite lubricante para un mantenimiento óptimo. Ideal para uso doméstico o profesional. ¡Consigue el estilo perfecto! ✂️
+Ficha técnica:
+Marca: IRM
+Modelo: 717
+Color: Negro y Plateado
+Dimensiones: 18.5 cm de largo, 5.8 cm de ancho
+Incluye:
+Cortadora de cabello
+4 Peines guía
+Tijeras
+Peine
+Aceite lubricante
+Alimentación: Con cable
+Uso: Doméstico/Profesional
+📋 Ficha técnica:
+**
+Marca: IRM
+Modelo: 717
+Color: Negro y Plateado
+Dimensiones: 18.5 cm de largo, 5.8 cm de ancho
+Incluye:
+Cortadora de cabello
+4 Peines guía
+Tijeras
+Peine
+Aceite lubricante
+Alimentación: Con cable
+Uso: Doméstico/Profesional
+</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Nuevo</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058198/1_kltviq.jpg</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058198/2_tebexl.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058200/3_t1ldxv.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058200/4_yckgg4.jpg</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>5900</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>8990</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>2090</t>
+        </is>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>7990</t>
+        </is>
+      </c>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="AK18" t="inlineStr">
+        <is>
+          <t>cortadora de cabello, IRM 717, kit peluquería, cortapelos eléctrico, tijeras, peine, barbería en casa, cuidado personal, accesorio de cabello, cortadora profesional, peines guía, estilo de cabello, corte de hombre, set de peluquería, herramienta de corte, belleza, máquina cortar pelo, recortadora, accesorios peluquería, IRM Chile</t>
+        </is>
+      </c>
+      <c r="AL18" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058201/WhatsApp_Image_2025-04-07_at_1.37.42_PM_3_sylpm5.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>P020</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>7858816084997</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>8499</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Kit de Limpieza Pantalla Opula LCD 100ml</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Tecnología</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Montelameda</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Descripción: 🌟 Mantén tus pantallas impecables con el Kit de Limpieza Opula. Ideal para LCD, laptops y más.
+Botella de 100 ml fácil de usar.
+Incluye cepillo para una limpieza óptima.
+Seguro y efectivo en diversas superficies.
+¡Cuida lo que más valoras con Opula! 🌐✨
+📋 Ficha técnica:
+Marca: Opula
+Tipo: Kit de limpieza para pantalla
+Contenido: 100 ml de limpiador
+Accesorios: Cepillo de limpieza
+Dimensiones botella: 13.5 cm x 3.5 cm
+Uso: Pantallas LCD y otros dispositivos electrónicos
+</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Nuevo</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058201/1_qh4xbv.jpg</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058202/3_zurq5y.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058202/4_ck7la5.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058201/2_qxhqlr.jpg</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>1200</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>4990</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>2790</t>
+        </is>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>3990</t>
+        </is>
+      </c>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="AK19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> kit de limpieza, pantalla LCD, Opula, limpiador de pantalla, 100 ml, cepillo, seguro para pantallas, accesorios electrónicos, cuidado de pantallas, dispositivos, limpieza electrónica, limpieza segura, pantalla cristalina, pantalla impecable, pantalla limpia, laptop, celulares, tablet, mantenimiento, cuidado personal.</t>
+        </is>
+      </c>
+      <c r="AL19" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058202/IRM_gxh4rv.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>P021</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>7858816136252</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>13625</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>IRM</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Palo de Selfie Extensible con Control Remoto</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Tecnología</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Montelameda</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Palo de Selfie Extensible con Control Remoto
+📝 Descripción: 📸 Lleva tus selfies al siguiente nivel con nuestro Palo de Selfie T18! Con un diseño compacto y ligero, ofrece un control remoto fácil de usar para capturar los mejores momentos sin esfuerzo. Compatible con la mayoría de los smartphones, mide 30.5 cm de altura y solo 7.3 cm de ancho, ¡perfecto para transportar! Ideal para viajes, eventos y más. Calidad y conveniencia en un solo producto. 🌟
+📋 Ficha técnica:
+Modelo: T18
+Referencia: 13625
+Longitud: 30.5 cm
+Ancho: 7.3 cm
+Material: Plástico resistente
+Control Remoto: Incluido
+Compatibilidad: Universal
+Color: Negro
+</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Nuevo</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058203/1_ihg7tu.jpg</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058203/2_nftbc4.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058204/3_bjdqsa.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058204/4_bvyxbu.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058204/5_sdfo1l.jpg</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>5500</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>9990</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>3490</t>
+        </is>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>7990</t>
+        </is>
+      </c>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="AK20" t="inlineStr">
+        <is>
+          <t>selfie stick, palo de selfie, control remoto, fotografía, portátil, extensible, smartphone, accesorio, viaje, evento, MeidiMake, T18, fotografía móvil, gadget, compacto, ligero, universal, práctico, accesorio móvil, calidad</t>
+        </is>
+      </c>
+      <c r="AL20" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058204/IRM_z3tyqo.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>P022</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>7858816135903</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>13590</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>IRM</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Plancha de Mano Portátil HB609</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Hogar</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Montelameda</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+📝 Descripción: Descubre la facilidad de mantener tu ropa impecable con la Plancha de Mano Portátil MeidiMake HB-609. Ideal para viajes y uso diario. Su diseño compacto de 18x10x7 cm es perfecto para ahorrar espacio. Incluye un vaso medidor y base antideslizante. 🌟 ¡Lleva la comodidad a donde vayas!
+📋 Ficha técnica:
+Marca: MeidiMake
+Modelo: HB-609
+Dimensiones: 18 cm x 10 cm x 7 cm
+Enchufe: 2 pines
+Incluye: Base y vaso medidor
+Ideal para: Hogar y viajes
+Color: Negro y gris
+</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Nuevo</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058205/1_h4sn9n.jpg</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058205/2_reo1bo.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058206/3_jad1ba.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058206/4_nhmkae.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058206/5_c7j8pq.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058207/6_th1v02.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058207/7_xepf5v.jpg</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>13900</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>19990</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>4590</t>
+        </is>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>17990</t>
+        </is>
+      </c>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="AK21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> plancha de mano, plancha portátil, MeidiMake, HB-609, planchado fácil, ropa impecable, diseño compacto, plancha de viaje, plancha eléctrica, hogar, tecnología, accesorios del hogar, electrodoméstico, mantenimiento ropa, portátil, fácil de usar, comodidad, eficiencia, utilidad, viaje</t>
+        </is>
+      </c>
+      <c r="AL21" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058207/IRM_lnpdjk.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>P023</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>7858816136276</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>13627</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Trípode de Fotografía y Selfie 154cm</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Tecnología</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Montelameda</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Trípode de Fotografía y Selfie 154cm
+📝 Descripción: 📸 Mejora tus fotos con nuestro trípode MeidiMake. Con altura ajustable hasta 154 cm y base estable de 50 cm, es ideal para fotos profesionales o selfies. Diseño compacto y ligero, fácil de transportar. Compatible con cámaras y smartphones. ¡Captura cada momento con precisión y estilo! 🌟
+📋 Ficha técnica:
+Altura máxima: 154 cm
+Tamaño de base: 50 cm
+Color: Negro
+Material: Aluminio
+Compatible: Cámaras y smartphones
+Diseño: Plegable y portátil
+Marca: MeidiMake
+Modelo: N03</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Nuevo</t>
+        </is>
+      </c>
+      <c r="J22" s="7" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058208/2_jqjdlz.jpg</t>
+        </is>
+      </c>
+      <c r="K22" s="7" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058208/1_ho5og0.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058208/3_goeawe.jpg,https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058209/4_d00wji.jpg</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>9900</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>14990</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>3590</t>
+        </is>
+      </c>
+      <c r="AA22" t="inlineStr">
+        <is>
+          <t>12990</t>
+        </is>
+      </c>
+      <c r="AB22" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="AK22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> trípode fotografía, palo selfie, MeidiMake, soporte cámara, trípode profesional, fotografía portátil, trípode ajustable, selfie stick, trípode aluminio, trípode ligero, equipo fotografía, trípode smartphone, trípode estable, trípode compacto, trípode negro, fotografía profesional, accesorio cámara, estabilizador smartphone, trípode MeidiMake, trípode N03</t>
+        </is>
+      </c>
+      <c r="AL22" t="inlineStr">
+        <is>
+          <t>https://res.cloudinary.com/dkl4xbslu/image/upload/v1744058209/IRM_ersdup.jpg</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AD11" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AD15" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="J22" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K22" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>